<commit_message>
Modularizzazione del progetto Streamlit
</commit_message>
<xml_diff>
--- a/blocchi_multi_foglio.xlsx
+++ b/blocchi_multi_foglio.xlsx
@@ -2431,17 +2431,17 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>538088</t>
+          <t>531877</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>C.so Francia  10093 Collegno ( TO )</t>
+          <t>C.so Francia   10093 Collegno ( TO )</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>DueB Costruzioni srl</t>
+          <t>FIBE srl</t>
         </is>
       </c>
       <c r="F57" t="n">
@@ -2466,17 +2466,17 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>531877</t>
+          <t>538088</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>C.so Francia   10093 Collegno ( TO )</t>
+          <t>C.so Francia  10093 Collegno ( TO )</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>FIBE srl</t>
+          <t>DueB Costruzioni srl</t>
         </is>
       </c>
       <c r="F58" t="n">
@@ -8075,17 +8075,17 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>534138</t>
+          <t>534139</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>Via M. Callas  35020 Albignasego ( PD )</t>
+          <t>Via Callas  35020 Albignasego ( PD )</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Immobiliare San Bonaventura srl; assegnato</t>
+          <t>Edilbaraldo srl</t>
         </is>
       </c>
       <c r="F69" t="n">
@@ -8110,17 +8110,17 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>534139</t>
+          <t>534138</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>Via Callas  35020 Albignasego ( PD )</t>
+          <t>Via M. Callas  35020 Albignasego ( PD )</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Edilbaraldo srl</t>
+          <t>Immobiliare San Bonaventura srl; assegnato</t>
         </is>
       </c>
       <c r="F70" t="n">
@@ -12249,12 +12249,12 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>537153</t>
+          <t>542609</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>Via delle Americhe  48122 Ravenna ( RA )</t>
+          <t>V.le delle Americhe  48122 Ravenna ( RA )</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -12284,12 +12284,12 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>542609</t>
+          <t>537153</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>V.le delle Americhe  48122 Ravenna ( RA )</t>
+          <t>Via delle Americhe  48122 Ravenna ( RA )</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -12494,17 +12494,17 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>532124</t>
+          <t>539779</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Via Savio snc  47814 Bellaria-Igea Marina ( RN )</t>
+          <t>Via Ravenna ang. Via Savio   47814 Bellaria-Igea Marina ( RN )</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Pompili Daniele</t>
+          <t>Moma srl</t>
         </is>
       </c>
       <c r="F48" t="n">
@@ -12529,17 +12529,17 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>539779</t>
+          <t>532124</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Via Ravenna ang. Via Savio   47814 Bellaria-Igea Marina ( RN )</t>
+          <t>Via Savio snc  47814 Bellaria-Igea Marina ( RN )</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Moma srl</t>
+          <t>Pompili Daniele</t>
         </is>
       </c>
       <c r="F49" t="n">
@@ -12578,7 +12578,7 @@
         </is>
       </c>
       <c r="F50" t="n">
-        <v>86649</v>
+        <v>86688</v>
       </c>
       <c r="G50" t="n">
         <v>5</v>
@@ -12613,7 +12613,7 @@
         </is>
       </c>
       <c r="F51" t="n">
-        <v>88092</v>
+        <v>88131</v>
       </c>
       <c r="G51" t="n">
         <v>5</v>
@@ -12648,7 +12648,7 @@
         </is>
       </c>
       <c r="F52" t="n">
-        <v>89721</v>
+        <v>89760</v>
       </c>
       <c r="G52" t="n">
         <v>6</v>
@@ -12683,7 +12683,7 @@
         </is>
       </c>
       <c r="F53" t="n">
-        <v>91221</v>
+        <v>91260</v>
       </c>
       <c r="G53" t="n">
         <v>6</v>
@@ -12718,7 +12718,7 @@
         </is>
       </c>
       <c r="F54" t="n">
-        <v>92899</v>
+        <v>92938</v>
       </c>
       <c r="G54" t="n">
         <v>6</v>
@@ -12753,7 +12753,7 @@
         </is>
       </c>
       <c r="F55" t="n">
-        <v>94347</v>
+        <v>94386</v>
       </c>
       <c r="G55" t="n">
         <v>6</v>
@@ -12788,7 +12788,7 @@
         </is>
       </c>
       <c r="F56" t="n">
-        <v>95714</v>
+        <v>95753</v>
       </c>
       <c r="G56" t="n">
         <v>6</v>
@@ -12823,7 +12823,7 @@
         </is>
       </c>
       <c r="F57" t="n">
-        <v>96935</v>
+        <v>96974</v>
       </c>
       <c r="G57" t="n">
         <v>6</v>
@@ -12858,7 +12858,7 @@
         </is>
       </c>
       <c r="F58" t="n">
-        <v>98308</v>
+        <v>98347</v>
       </c>
       <c r="G58" t="n">
         <v>6</v>
@@ -12893,7 +12893,7 @@
         </is>
       </c>
       <c r="F59" t="n">
-        <v>99823</v>
+        <v>99862</v>
       </c>
       <c r="G59" t="n">
         <v>6</v>
@@ -12928,7 +12928,7 @@
         </is>
       </c>
       <c r="F60" t="n">
-        <v>101632</v>
+        <v>101671</v>
       </c>
       <c r="G60" t="n">
         <v>6</v>
@@ -12963,7 +12963,7 @@
         </is>
       </c>
       <c r="F61" t="n">
-        <v>103593</v>
+        <v>103632</v>
       </c>
       <c r="G61" t="n">
         <v>6</v>
@@ -12998,7 +12998,7 @@
         </is>
       </c>
       <c r="F62" t="n">
-        <v>104968</v>
+        <v>105007</v>
       </c>
       <c r="G62" t="n">
         <v>7</v>
@@ -13033,7 +13033,7 @@
         </is>
       </c>
       <c r="F63" t="n">
-        <v>106452</v>
+        <v>106491</v>
       </c>
       <c r="G63" t="n">
         <v>7</v>
@@ -13068,7 +13068,7 @@
         </is>
       </c>
       <c r="F64" t="n">
-        <v>108550</v>
+        <v>108589</v>
       </c>
       <c r="G64" t="n">
         <v>7</v>
@@ -13103,7 +13103,7 @@
         </is>
       </c>
       <c r="F65" t="n">
-        <v>110094</v>
+        <v>110133</v>
       </c>
       <c r="G65" t="n">
         <v>7</v>
@@ -13138,7 +13138,7 @@
         </is>
       </c>
       <c r="F66" t="n">
-        <v>111695</v>
+        <v>111734</v>
       </c>
       <c r="G66" t="n">
         <v>7</v>
@@ -13173,7 +13173,7 @@
         </is>
       </c>
       <c r="F67" t="n">
-        <v>113681</v>
+        <v>113720</v>
       </c>
       <c r="G67" t="n">
         <v>7</v>
@@ -13208,7 +13208,7 @@
         </is>
       </c>
       <c r="F68" t="n">
-        <v>115243</v>
+        <v>115282</v>
       </c>
       <c r="G68" t="n">
         <v>7</v>
@@ -13243,7 +13243,7 @@
         </is>
       </c>
       <c r="F69" t="n">
-        <v>117010</v>
+        <v>117049</v>
       </c>
       <c r="G69" t="n">
         <v>7</v>
@@ -13278,7 +13278,7 @@
         </is>
       </c>
       <c r="F70" t="n">
-        <v>118626</v>
+        <v>118665</v>
       </c>
       <c r="G70" t="n">
         <v>7</v>
@@ -13313,7 +13313,7 @@
         </is>
       </c>
       <c r="F71" t="n">
-        <v>121480</v>
+        <v>121519</v>
       </c>
       <c r="G71" t="n">
         <v>7</v>
@@ -13348,7 +13348,7 @@
         </is>
       </c>
       <c r="F72" t="n">
-        <v>125844</v>
+        <v>125883</v>
       </c>
       <c r="G72" t="n">
         <v>8</v>
@@ -13383,7 +13383,7 @@
         </is>
       </c>
       <c r="F73" t="n">
-        <v>129167</v>
+        <v>129206</v>
       </c>
       <c r="G73" t="n">
         <v>8</v>
@@ -13418,7 +13418,7 @@
         </is>
       </c>
       <c r="F74" t="n">
-        <v>129167</v>
+        <v>129206</v>
       </c>
       <c r="G74" t="n">
         <v>8</v>
@@ -13453,7 +13453,7 @@
         </is>
       </c>
       <c r="F75" t="n">
-        <v>131484</v>
+        <v>131523</v>
       </c>
       <c r="G75" t="n">
         <v>8</v>
@@ -13488,7 +13488,7 @@
         </is>
       </c>
       <c r="F76" t="n">
-        <v>134496</v>
+        <v>134535</v>
       </c>
       <c r="G76" t="n">
         <v>8</v>
@@ -13523,7 +13523,7 @@
         </is>
       </c>
       <c r="F77" t="n">
-        <v>136320</v>
+        <v>136359</v>
       </c>
       <c r="G77" t="n">
         <v>8</v>
@@ -13558,7 +13558,7 @@
         </is>
       </c>
       <c r="F78" t="n">
-        <v>137520</v>
+        <v>137559</v>
       </c>
       <c r="G78" t="n">
         <v>8</v>
@@ -13593,7 +13593,7 @@
         </is>
       </c>
       <c r="F79" t="n">
-        <v>139185</v>
+        <v>139224</v>
       </c>
       <c r="G79" t="n">
         <v>8</v>
@@ -13628,7 +13628,7 @@
         </is>
       </c>
       <c r="F80" t="n">
-        <v>141237</v>
+        <v>141276</v>
       </c>
       <c r="G80" t="n">
         <v>8</v>
@@ -13663,7 +13663,7 @@
         </is>
       </c>
       <c r="F81" t="n">
-        <v>142437</v>
+        <v>142476</v>
       </c>
       <c r="G81" t="n">
         <v>8</v>
@@ -13698,7 +13698,7 @@
         </is>
       </c>
       <c r="F82" t="n">
-        <v>143832</v>
+        <v>143871</v>
       </c>
       <c r="G82" t="n">
         <v>9</v>
@@ -13733,7 +13733,7 @@
         </is>
       </c>
       <c r="F83" t="n">
-        <v>145700</v>
+        <v>145739</v>
       </c>
       <c r="G83" t="n">
         <v>9</v>
@@ -13768,7 +13768,7 @@
         </is>
       </c>
       <c r="F84" t="n">
-        <v>148221</v>
+        <v>148260</v>
       </c>
       <c r="G84" t="n">
         <v>9</v>
@@ -13803,7 +13803,7 @@
         </is>
       </c>
       <c r="F85" t="n">
-        <v>150524</v>
+        <v>150563</v>
       </c>
       <c r="G85" t="n">
         <v>9</v>
@@ -13838,7 +13838,7 @@
         </is>
       </c>
       <c r="F86" t="n">
-        <v>152622</v>
+        <v>152661</v>
       </c>
       <c r="G86" t="n">
         <v>9</v>
@@ -13873,7 +13873,7 @@
         </is>
       </c>
       <c r="F87" t="n">
-        <v>154304</v>
+        <v>154343</v>
       </c>
       <c r="G87" t="n">
         <v>9</v>
@@ -13908,7 +13908,7 @@
         </is>
       </c>
       <c r="F88" t="n">
-        <v>156713</v>
+        <v>156752</v>
       </c>
       <c r="G88" t="n">
         <v>9</v>
@@ -13943,7 +13943,7 @@
         </is>
       </c>
       <c r="F89" t="n">
-        <v>159109</v>
+        <v>159148</v>
       </c>
       <c r="G89" t="n">
         <v>9</v>
@@ -13978,7 +13978,7 @@
         </is>
       </c>
       <c r="F90" t="n">
-        <v>160867</v>
+        <v>160906</v>
       </c>
       <c r="G90" t="n">
         <v>9</v>
@@ -14013,7 +14013,7 @@
         </is>
       </c>
       <c r="F91" t="n">
-        <v>162544</v>
+        <v>162583</v>
       </c>
       <c r="G91" t="n">
         <v>9</v>
@@ -14048,7 +14048,7 @@
         </is>
       </c>
       <c r="F92" t="n">
-        <v>164228</v>
+        <v>164267</v>
       </c>
       <c r="G92" t="n">
         <v>10</v>
@@ -14083,7 +14083,7 @@
         </is>
       </c>
       <c r="F93" t="n">
-        <v>165503</v>
+        <v>165542</v>
       </c>
       <c r="G93" t="n">
         <v>10</v>
@@ -14118,7 +14118,7 @@
         </is>
       </c>
       <c r="F94" t="n">
-        <v>167151</v>
+        <v>167190</v>
       </c>
       <c r="G94" t="n">
         <v>10</v>
@@ -14153,7 +14153,7 @@
         </is>
       </c>
       <c r="F95" t="n">
-        <v>169267</v>
+        <v>169306</v>
       </c>
       <c r="G95" t="n">
         <v>10</v>
@@ -14188,7 +14188,7 @@
         </is>
       </c>
       <c r="F96" t="n">
-        <v>171867</v>
+        <v>171906</v>
       </c>
       <c r="G96" t="n">
         <v>10</v>
@@ -14223,7 +14223,7 @@
         </is>
       </c>
       <c r="F97" t="n">
-        <v>173798</v>
+        <v>173837</v>
       </c>
       <c r="G97" t="n">
         <v>10</v>
@@ -14258,7 +14258,7 @@
         </is>
       </c>
       <c r="F98" t="n">
-        <v>175101</v>
+        <v>175140</v>
       </c>
       <c r="G98" t="n">
         <v>10</v>
@@ -14293,7 +14293,7 @@
         </is>
       </c>
       <c r="F99" t="n">
-        <v>176475</v>
+        <v>176514</v>
       </c>
       <c r="G99" t="n">
         <v>10</v>
@@ -14328,7 +14328,7 @@
         </is>
       </c>
       <c r="F100" t="n">
-        <v>177675</v>
+        <v>177714</v>
       </c>
       <c r="G100" t="n">
         <v>10</v>
@@ -14363,7 +14363,7 @@
         </is>
       </c>
       <c r="F101" t="n">
-        <v>179104</v>
+        <v>179143</v>
       </c>
       <c r="G101" t="n">
         <v>10</v>
@@ -14398,7 +14398,7 @@
         </is>
       </c>
       <c r="F102" t="n">
-        <v>180370</v>
+        <v>180409</v>
       </c>
       <c r="G102" t="n">
         <v>11</v>
@@ -14433,7 +14433,7 @@
         </is>
       </c>
       <c r="F103" t="n">
-        <v>181884</v>
+        <v>181923</v>
       </c>
       <c r="G103" t="n">
         <v>11</v>
@@ -14468,7 +14468,7 @@
         </is>
       </c>
       <c r="F104" t="n">
-        <v>183567</v>
+        <v>183606</v>
       </c>
       <c r="G104" t="n">
         <v>11</v>
@@ -14503,7 +14503,7 @@
         </is>
       </c>
       <c r="F105" t="n">
-        <v>185075</v>
+        <v>185114</v>
       </c>
       <c r="G105" t="n">
         <v>11</v>
@@ -14538,7 +14538,7 @@
         </is>
       </c>
       <c r="F106" t="n">
-        <v>186694</v>
+        <v>186733</v>
       </c>
       <c r="G106" t="n">
         <v>11</v>
@@ -14573,7 +14573,7 @@
         </is>
       </c>
       <c r="F107" t="n">
-        <v>188626</v>
+        <v>188665</v>
       </c>
       <c r="G107" t="n">
         <v>11</v>
@@ -14608,7 +14608,7 @@
         </is>
       </c>
       <c r="F108" t="n">
-        <v>190268</v>
+        <v>190307</v>
       </c>
       <c r="G108" t="n">
         <v>11</v>
@@ -14643,7 +14643,7 @@
         </is>
       </c>
       <c r="F109" t="n">
-        <v>191660</v>
+        <v>191699</v>
       </c>
       <c r="G109" t="n">
         <v>11</v>
@@ -14678,7 +14678,7 @@
         </is>
       </c>
       <c r="F110" t="n">
-        <v>193039</v>
+        <v>193078</v>
       </c>
       <c r="G110" t="n">
         <v>11</v>
@@ -14713,7 +14713,7 @@
         </is>
       </c>
       <c r="F111" t="n">
-        <v>195334</v>
+        <v>195373</v>
       </c>
       <c r="G111" t="n">
         <v>11</v>
@@ -14748,7 +14748,7 @@
         </is>
       </c>
       <c r="F112" t="n">
-        <v>197521</v>
+        <v>197560</v>
       </c>
       <c r="G112" t="n">
         <v>12</v>
@@ -14783,7 +14783,7 @@
         </is>
       </c>
       <c r="F113" t="n">
-        <v>199832</v>
+        <v>199871</v>
       </c>
       <c r="G113" t="n">
         <v>12</v>
@@ -14818,7 +14818,7 @@
         </is>
       </c>
       <c r="F114" t="n">
-        <v>201167</v>
+        <v>201206</v>
       </c>
       <c r="G114" t="n">
         <v>12</v>
@@ -14853,7 +14853,7 @@
         </is>
       </c>
       <c r="F115" t="n">
-        <v>202888</v>
+        <v>202927</v>
       </c>
       <c r="G115" t="n">
         <v>12</v>
@@ -14888,7 +14888,7 @@
         </is>
       </c>
       <c r="F116" t="n">
-        <v>204739</v>
+        <v>204778</v>
       </c>
       <c r="G116" t="n">
         <v>12</v>
@@ -14923,7 +14923,7 @@
         </is>
       </c>
       <c r="F117" t="n">
-        <v>206134</v>
+        <v>206173</v>
       </c>
       <c r="G117" t="n">
         <v>12</v>
@@ -14958,7 +14958,7 @@
         </is>
       </c>
       <c r="F118" t="n">
-        <v>207634</v>
+        <v>207673</v>
       </c>
       <c r="G118" t="n">
         <v>12</v>
@@ -14993,7 +14993,7 @@
         </is>
       </c>
       <c r="F119" t="n">
-        <v>209467</v>
+        <v>209506</v>
       </c>
       <c r="G119" t="n">
         <v>12</v>
@@ -15028,7 +15028,7 @@
         </is>
       </c>
       <c r="F120" t="n">
-        <v>212142</v>
+        <v>212181</v>
       </c>
       <c r="G120" t="n">
         <v>12</v>
@@ -15063,7 +15063,7 @@
         </is>
       </c>
       <c r="F121" t="n">
-        <v>214272</v>
+        <v>214311</v>
       </c>
       <c r="G121" t="n">
         <v>12</v>
@@ -15098,7 +15098,7 @@
         </is>
       </c>
       <c r="F122" t="n">
-        <v>216252</v>
+        <v>216291</v>
       </c>
       <c r="G122" t="n">
         <v>13</v>
@@ -15133,7 +15133,7 @@
         </is>
       </c>
       <c r="F123" t="n">
-        <v>218132</v>
+        <v>218171</v>
       </c>
       <c r="G123" t="n">
         <v>13</v>
@@ -15168,7 +15168,7 @@
         </is>
       </c>
       <c r="F124" t="n">
-        <v>220124</v>
+        <v>220163</v>
       </c>
       <c r="G124" t="n">
         <v>13</v>
@@ -15203,7 +15203,7 @@
         </is>
       </c>
       <c r="F125" t="n">
-        <v>221954</v>
+        <v>221993</v>
       </c>
       <c r="G125" t="n">
         <v>13</v>
@@ -15238,7 +15238,7 @@
         </is>
       </c>
       <c r="F126" t="n">
-        <v>223941</v>
+        <v>223980</v>
       </c>
       <c r="G126" t="n">
         <v>13</v>
@@ -15273,7 +15273,7 @@
         </is>
       </c>
       <c r="F127" t="n">
-        <v>226703</v>
+        <v>226742</v>
       </c>
       <c r="G127" t="n">
         <v>13</v>
@@ -15308,7 +15308,7 @@
         </is>
       </c>
       <c r="F128" t="n">
-        <v>229274</v>
+        <v>229313</v>
       </c>
       <c r="G128" t="n">
         <v>13</v>
@@ -15343,7 +15343,7 @@
         </is>
       </c>
       <c r="F129" t="n">
-        <v>230952</v>
+        <v>230991</v>
       </c>
       <c r="G129" t="n">
         <v>13</v>
@@ -15378,7 +15378,7 @@
         </is>
       </c>
       <c r="F130" t="n">
-        <v>232294</v>
+        <v>232333</v>
       </c>
       <c r="G130" t="n">
         <v>13</v>
@@ -15413,7 +15413,7 @@
         </is>
       </c>
       <c r="F131" t="n">
-        <v>236764</v>
+        <v>236803</v>
       </c>
       <c r="G131" t="n">
         <v>13</v>
@@ -15448,7 +15448,7 @@
         </is>
       </c>
       <c r="F132" t="n">
-        <v>239257</v>
+        <v>239296</v>
       </c>
       <c r="G132" t="n">
         <v>14</v>
@@ -15483,7 +15483,7 @@
         </is>
       </c>
       <c r="F133" t="n">
-        <v>240457</v>
+        <v>240496</v>
       </c>
       <c r="G133" t="n">
         <v>14</v>
@@ -15518,7 +15518,7 @@
         </is>
       </c>
       <c r="F134" t="n">
-        <v>244383</v>
+        <v>244422</v>
       </c>
       <c r="G134" t="n">
         <v>14</v>
@@ -15553,7 +15553,7 @@
         </is>
       </c>
       <c r="F135" t="n">
-        <v>245652</v>
+        <v>245691</v>
       </c>
       <c r="G135" t="n">
         <v>14</v>
@@ -15588,7 +15588,7 @@
         </is>
       </c>
       <c r="F136" t="n">
-        <v>248388</v>
+        <v>248427</v>
       </c>
       <c r="G136" t="n">
         <v>14</v>
@@ -15623,7 +15623,7 @@
         </is>
       </c>
       <c r="F137" t="n">
-        <v>252010</v>
+        <v>252049</v>
       </c>
       <c r="G137" t="n">
         <v>14</v>
@@ -15658,7 +15658,7 @@
         </is>
       </c>
       <c r="F138" t="n">
-        <v>253653</v>
+        <v>253692</v>
       </c>
       <c r="G138" t="n">
         <v>14</v>
@@ -15693,7 +15693,7 @@
         </is>
       </c>
       <c r="F139" t="n">
-        <v>255179</v>
+        <v>255218</v>
       </c>
       <c r="G139" t="n">
         <v>14</v>
@@ -15728,7 +15728,7 @@
         </is>
       </c>
       <c r="F140" t="n">
-        <v>256631</v>
+        <v>256670</v>
       </c>
       <c r="G140" t="n">
         <v>14</v>

</xml_diff>